<commit_message>
sql de un solo archivo nuevo, xls tambien actualizado
</commit_message>
<xml_diff>
--- a/src/database/der_move_zapatillas.xlsx
+++ b/src/database/der_move_zapatillas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -37,9 +37,6 @@
     <t>MOVE // TIENDA ZAPATILLAS</t>
   </si>
   <si>
-    <t>(user/admin)</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -61,12 +58,6 @@
     <t>users</t>
   </si>
   <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -82,21 +73,12 @@
     <t>brands</t>
   </si>
   <si>
-    <t>(adidas/nike/etc)</t>
-  </si>
-  <si>
     <t>id_product</t>
   </si>
   <si>
     <t>id_user</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>pay</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -118,9 +100,6 @@
     <t>date_create</t>
   </si>
   <si>
-    <t>date_modif</t>
-  </si>
-  <si>
     <t>( male / female )</t>
   </si>
   <si>
@@ -143,13 +122,43 @@
   </si>
   <si>
     <t>gender</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>date_update</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>OBS: No se agrego tablas de…</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>( user / admin )</t>
+  </si>
+  <si>
+    <t>( adidas / nike / etc )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +178,21 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -272,6 +296,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,6 +511,51 @@
         <a:xfrm>
           <a:off x="2211917" y="1767417"/>
           <a:ext cx="2804583" cy="751416"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>42333</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95253</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>740834</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>84668</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="6 Conector recto"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5984876" y="2989793"/>
+          <a:ext cx="1703915" cy="698501"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -796,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L23"/>
+  <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -822,64 +893,73 @@
     <row r="2" spans="2:12" ht="26.25">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
+      <c r="F2" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="K3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="F4" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="K4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:12">
       <c r="K5" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:12">
       <c r="K6" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:12">
       <c r="K7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:12">
       <c r="H8" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -887,76 +967,91 @@
         <v>0</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C11" s="10"/>
       <c r="H11" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="L11" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="H12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" t="s">
-        <v>4</v>
+      <c r="F12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="F13" s="3" t="s">
-        <v>3</v>
+      <c r="F13" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="I13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="10"/>
       <c r="F14" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="2:12">
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="10"/>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>5</v>
@@ -967,77 +1062,72 @@
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
+    </row>
+    <row r="20" spans="2:8">
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
       <c r="B21" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C21" s="10"/>
       <c r="F21" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:8">
       <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="C23" s="10"/>
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>